<commit_message>
Ssbv: handle by open another table
</commit_message>
<xml_diff>
--- a/java/bundles/org.eclipse.set.feature/rootdir/data/export/excel/ssbv_vorlage.xlsx
+++ b/java/bundles/org.eclipse.set.feature/rootdir/data/export/excel/ssbv_vorlage.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\eclipse\sbider\data\export\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1E125318-41C6-44FA-9386-0C50ACA51A3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F1EFE09-F387-46D8-ACCB-D0F57995F65B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sskz" sheetId="6" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sskz!$A$1:$D$52</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sskz!$A$1:$C$52</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">Sskz!$1:$4</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
@@ -24,12 +24,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>A</t>
-  </si>
-  <si>
-    <t>C</t>
   </si>
   <si>
     <t>B</t>
@@ -40,9 +37,6 @@
   </si>
   <si>
     <t>Referenziert von Objekt</t>
-  </si>
-  <si>
-    <t>Ausgabe in Plan</t>
   </si>
 </sst>
 </file>
@@ -71,7 +65,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -129,11 +123,24 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -160,6 +167,9 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -466,43 +476,39 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:AP52"/>
+  <dimension ref="B1:AO52"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B3"/>
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.85546875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="138.7109375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="24" style="2" customWidth="1"/>
-    <col min="4" max="4" width="25.140625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="11.85546875" style="2" customWidth="1"/>
-    <col min="6" max="6" width="12" style="2" customWidth="1"/>
-    <col min="7" max="7" width="11.85546875" style="2" customWidth="1"/>
-    <col min="8" max="8" width="15.5703125" style="2" customWidth="1"/>
-    <col min="9" max="9" width="9" style="2" customWidth="1"/>
-    <col min="10" max="10" width="50.28515625" style="2" customWidth="1"/>
-    <col min="11" max="11" width="7.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="7.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="5.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="11" style="2" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.42578125" style="2"/>
-    <col min="17" max="17" width="14.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="18" max="16384" width="11.42578125" style="2"/>
+    <col min="2" max="3" width="33.7109375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="12" style="2" customWidth="1"/>
+    <col min="6" max="6" width="11.85546875" style="2" customWidth="1"/>
+    <col min="7" max="7" width="15.5703125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="9" style="2" customWidth="1"/>
+    <col min="9" max="9" width="50.28515625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="7.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="11" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.42578125" style="2"/>
+    <col min="16" max="16" width="14.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="17" max="16384" width="11.42578125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:42" s="1" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:41" s="1" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="5" t="s">
+      <c r="C1" s="10" t="s">
         <v>1</v>
       </c>
+      <c r="D1" s="2"/>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
@@ -540,302 +546,295 @@
       <c r="AM1" s="2"/>
       <c r="AN1" s="2"/>
       <c r="AO1" s="2"/>
-      <c r="AP1" s="2"/>
-    </row>
-    <row r="2" spans="2:42" ht="37.700000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="2:41" ht="37.700000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>5</v>
-      </c>
+      <c r="G2" s="3"/>
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
       <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-    </row>
-    <row r="3" spans="2:42" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="2:41" x14ac:dyDescent="0.25">
       <c r="B3" s="9"/>
       <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="F3" s="3"/>
-      <c r="K3" s="3"/>
-    </row>
-    <row r="4" spans="2:42" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E3" s="3"/>
+      <c r="J3" s="3"/>
+    </row>
+    <row r="4" spans="2:41" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="7"/>
       <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-    </row>
-    <row r="5" spans="2:42" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="2:41" x14ac:dyDescent="0.25">
       <c r="B5" s="4"/>
+      <c r="E5" s="4"/>
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
       <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-    </row>
-    <row r="6" spans="2:42" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="2:41" x14ac:dyDescent="0.25">
       <c r="B6" s="4"/>
+      <c r="E6" s="4"/>
       <c r="F6" s="4"/>
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
-    </row>
-    <row r="7" spans="2:42" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="2:41" x14ac:dyDescent="0.25">
       <c r="B7" s="4"/>
+      <c r="E7" s="4"/>
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-    </row>
-    <row r="8" spans="2:42" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="2:41" x14ac:dyDescent="0.25">
       <c r="B8" s="4"/>
+      <c r="E8" s="4"/>
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-    </row>
-    <row r="9" spans="2:42" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="2:41" x14ac:dyDescent="0.25">
       <c r="B9" s="4"/>
+      <c r="E9" s="4"/>
       <c r="F9" s="4"/>
       <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-    </row>
-    <row r="10" spans="2:42" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="2:41" x14ac:dyDescent="0.25">
       <c r="B10" s="4"/>
+      <c r="E10" s="4"/>
       <c r="F10" s="4"/>
       <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
-    </row>
-    <row r="11" spans="2:42" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="2:41" x14ac:dyDescent="0.25">
       <c r="B11" s="4"/>
+      <c r="E11" s="4"/>
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
-    </row>
-    <row r="12" spans="2:42" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="2:41" x14ac:dyDescent="0.25">
       <c r="B12" s="4"/>
+      <c r="E12" s="4"/>
       <c r="F12" s="4"/>
       <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
-    </row>
-    <row r="13" spans="2:42" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="2:41" x14ac:dyDescent="0.25">
       <c r="B13" s="4"/>
+      <c r="E13" s="4"/>
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
-    </row>
-    <row r="14" spans="2:42" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="2:41" x14ac:dyDescent="0.25">
       <c r="B14" s="4"/>
+      <c r="E14" s="4"/>
       <c r="F14" s="4"/>
       <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
-    </row>
-    <row r="15" spans="2:42" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="2:41" x14ac:dyDescent="0.25">
       <c r="B15" s="4"/>
+      <c r="E15" s="4"/>
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
-    </row>
-    <row r="16" spans="2:42" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="2:41" x14ac:dyDescent="0.25">
       <c r="B16" s="4"/>
+      <c r="E16" s="4"/>
       <c r="F16" s="4"/>
       <c r="G16" s="4"/>
-      <c r="H16" s="4"/>
-    </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" s="4"/>
+      <c r="E17" s="4"/>
       <c r="F17" s="4"/>
       <c r="G17" s="4"/>
-      <c r="H17" s="4"/>
-    </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" s="4"/>
+      <c r="E18" s="4"/>
       <c r="F18" s="4"/>
       <c r="G18" s="4"/>
-      <c r="H18" s="4"/>
-    </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" s="4"/>
+      <c r="E19" s="4"/>
       <c r="F19" s="4"/>
       <c r="G19" s="4"/>
-      <c r="H19" s="4"/>
-    </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" s="4"/>
+      <c r="E20" s="4"/>
       <c r="F20" s="4"/>
       <c r="G20" s="4"/>
-      <c r="H20" s="4"/>
-    </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" s="4"/>
+      <c r="E21" s="4"/>
       <c r="F21" s="4"/>
       <c r="G21" s="4"/>
-      <c r="H21" s="4"/>
-    </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" s="4"/>
+      <c r="E22" s="4"/>
       <c r="F22" s="4"/>
       <c r="G22" s="4"/>
-      <c r="H22" s="4"/>
-    </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23" s="4"/>
+      <c r="E23" s="4"/>
       <c r="F23" s="4"/>
       <c r="G23" s="4"/>
-      <c r="H23" s="4"/>
-    </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="E24" s="4"/>
       <c r="F24" s="4"/>
       <c r="G24" s="4"/>
-      <c r="H24" s="4"/>
-    </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="E25" s="4"/>
       <c r="F25" s="4"/>
       <c r="G25" s="4"/>
-      <c r="H25" s="4"/>
-    </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="E26" s="4"/>
       <c r="F26" s="4"/>
       <c r="G26" s="4"/>
-      <c r="H26" s="4"/>
-    </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="E27" s="4"/>
       <c r="F27" s="4"/>
       <c r="G27" s="4"/>
-      <c r="H27" s="4"/>
-    </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="E28" s="4"/>
       <c r="F28" s="4"/>
       <c r="G28" s="4"/>
-      <c r="H28" s="4"/>
-    </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="E29" s="4"/>
       <c r="F29" s="4"/>
       <c r="G29" s="4"/>
-      <c r="H29" s="4"/>
-    </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="E30" s="4"/>
       <c r="F30" s="4"/>
       <c r="G30" s="4"/>
-      <c r="H30" s="4"/>
-    </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="E31" s="4"/>
       <c r="F31" s="4"/>
       <c r="G31" s="4"/>
-      <c r="H31" s="4"/>
-    </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="E32" s="4"/>
       <c r="F32" s="4"/>
       <c r="G32" s="4"/>
-      <c r="H32" s="4"/>
-    </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="E33" s="4"/>
       <c r="F33" s="4"/>
       <c r="G33" s="4"/>
-      <c r="H33" s="4"/>
-    </row>
-    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B34" s="3"/>
+      <c r="E34" s="4"/>
       <c r="F34" s="4"/>
       <c r="G34" s="4"/>
-      <c r="H34" s="4"/>
-    </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="E35" s="4"/>
       <c r="F35" s="4"/>
       <c r="G35" s="4"/>
-      <c r="H35" s="4"/>
-    </row>
-    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="E36" s="4"/>
       <c r="F36" s="4"/>
       <c r="G36" s="4"/>
-      <c r="H36" s="4"/>
-    </row>
-    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="E37" s="4"/>
       <c r="F37" s="4"/>
       <c r="G37" s="4"/>
-      <c r="H37" s="4"/>
-    </row>
-    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="E38" s="4"/>
       <c r="F38" s="4"/>
       <c r="G38" s="4"/>
-      <c r="H38" s="4"/>
-    </row>
-    <row r="39" spans="2:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="E39" s="4"/>
       <c r="F39" s="4"/>
       <c r="G39" s="4"/>
-      <c r="H39" s="4"/>
-    </row>
-    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="E40" s="4"/>
       <c r="F40" s="4"/>
       <c r="G40" s="4"/>
-      <c r="H40" s="4"/>
-    </row>
-    <row r="41" spans="2:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="E41" s="4"/>
       <c r="F41" s="4"/>
       <c r="G41" s="4"/>
-      <c r="H41" s="4"/>
-    </row>
-    <row r="42" spans="2:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="42" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="E42" s="4"/>
       <c r="F42" s="4"/>
       <c r="G42" s="4"/>
-      <c r="H42" s="4"/>
-    </row>
-    <row r="43" spans="2:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="43" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="E43" s="4"/>
       <c r="F43" s="4"/>
       <c r="G43" s="4"/>
-      <c r="H43" s="4"/>
-    </row>
-    <row r="44" spans="2:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="44" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="E44" s="4"/>
       <c r="F44" s="4"/>
       <c r="G44" s="4"/>
-      <c r="H44" s="4"/>
-    </row>
-    <row r="45" spans="2:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="45" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="E45" s="4"/>
       <c r="F45" s="4"/>
       <c r="G45" s="4"/>
-      <c r="H45" s="4"/>
-    </row>
-    <row r="46" spans="2:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="46" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="E46" s="4"/>
       <c r="F46" s="4"/>
       <c r="G46" s="4"/>
-      <c r="H46" s="4"/>
-    </row>
-    <row r="47" spans="2:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="47" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="E47" s="4"/>
       <c r="F47" s="4"/>
       <c r="G47" s="4"/>
-      <c r="H47" s="4"/>
-    </row>
-    <row r="48" spans="2:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="48" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="E48" s="4"/>
       <c r="F48" s="4"/>
       <c r="G48" s="4"/>
-      <c r="H48" s="4"/>
-    </row>
-    <row r="49" spans="6:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="49" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E49" s="4"/>
       <c r="F49" s="4"/>
       <c r="G49" s="4"/>
-      <c r="H49" s="4"/>
-    </row>
-    <row r="50" spans="6:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="50" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E50" s="4"/>
       <c r="F50" s="4"/>
       <c r="G50" s="4"/>
-      <c r="H50" s="4"/>
-    </row>
-    <row r="51" spans="6:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="51" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E51" s="4"/>
       <c r="F51" s="4"/>
       <c r="G51" s="4"/>
-      <c r="H51" s="4"/>
-    </row>
-    <row r="52" spans="6:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="52" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E52" s="4"/>
       <c r="F52" s="4"/>
       <c r="G52" s="4"/>
-      <c r="H52" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="2">
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
   </mergeCells>
   <printOptions gridLines="1"/>
   <pageMargins left="0.78740157480314965" right="0.39370078740157483" top="0.19685039370078741" bottom="0.59055118110236227" header="0" footer="0"/>

</xml_diff>